<commit_message>
Fixed minor table formatting
Calibri 11 all over.
</commit_message>
<xml_diff>
--- a/Output/Tables/TD_SubTypes_Tables.xlsx
+++ b/Output/Tables/TD_SubTypes_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CABM\CINJ\TD_subtype\Output\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9071E1-265E-417E-9959-664C4132D007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DFAA0C-A9D6-4B6E-9203-76D9FC91BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="17760" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS Subtypes Tables" sheetId="1" r:id="rId1"/>
@@ -153,18 +153,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -282,75 +281,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -359,30 +361,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -398,29 +382,10 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -436,29 +401,10 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -474,28 +420,39 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="medium">
           <color indexed="64"/>
         </top>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -509,13 +466,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -528,8 +485,6 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -543,13 +498,109 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="medium">
           <color indexed="64"/>
@@ -560,8 +611,6 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -586,6 +635,17 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+      </font>
     </dxf>
     <dxf>
       <border>
@@ -605,13 +665,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -620,12 +680,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -642,15 +696,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A3:F23" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D8FDF88-7DBA-4F2F-B11E-B8A77BB223B0}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:B2" xr:uid="{6D8FDF88-7DBA-4F2F-B11E-B8A77BB223B0}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{0B949021-5E8F-412F-B9CE-821C3002F88E}" name="Tables for TD Subtype Paper" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{5C2006AE-05FA-4835-8DF9-2F869D67DB9F}" name="Tab" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A3:F23" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A3:F23" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Kmclust" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Kmsize+" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="BHCclust" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="BHCsize*" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Pos. Correlation" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Neg. Correlation" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Kmclust" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Kmsize+" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="BHCclust" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="BHCsize*" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Pos. Correlation" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Neg. Correlation" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -980,28 +1045,31 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="52.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="22" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1010,7 +1078,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1030,283 +1098,283 @@
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="6">
+    <row r="4" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <v>210</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="9">
         <v>6</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="9">
         <v>249</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="17" t="s">
+    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8" t="s">
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="6">
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="9">
         <v>40</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="12" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7">
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9">
         <v>3</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="9">
         <v>30</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7">
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9">
         <v>4</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="9">
         <v>10</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="6">
+    <row r="14" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="8">
         <v>3</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="9">
         <v>289</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="9">
         <v>5</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="9">
         <v>250</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="20" t="s">
+    <row r="15" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="20" t="s">
+    <row r="16" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="6">
+      <c r="F16" s="20"/>
+    </row>
+    <row r="17" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="8">
         <v>4</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="9">
         <v>229</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="9">
         <v>2</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="9">
         <v>206</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="20" t="s">
+    <row r="18" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="8" t="s">
+    <row r="19" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="10" t="s">
+    <row r="20" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="6">
+    <row r="21" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="8">
         <v>5</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="9">
         <v>97</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="9">
         <v>1</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="9">
         <v>120</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8" t="s">
+    <row r="22" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="19" t="s">
+    <row r="23" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1319,12 +1387,12 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>